<commit_message>
Write to openxlsx over writexl
</commit_message>
<xml_diff>
--- a/20240123_Excel_readxl/data/Summarized_Data.xlsx
+++ b/20240123_Excel_readxl/data/Summarized_Data.xlsx
@@ -1,32 +1,55 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t xml:space="preserve">Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Media</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avg_Norm_Fluor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sd_Norm_Fluor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WT</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -52,17 +75,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -112,10 +131,6 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -141,15 +156,12 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -175,6 +187,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -350,293 +363,236 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Time</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Strain</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Media</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Avg_Norm_Fluor</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Sd_Norm_Fluor</t>
-        </is>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2">
+      <c r="A2" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Mut</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>LB</t>
-        </is>
-      </c>
-      <c r="D2">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="n">
         <v>13.625</v>
       </c>
-      <c r="E2">
-        <v>10.12731455026455</v>
+      <c r="E2" t="n">
+        <v>10.1273145502645</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3">
+      <c r="A3" t="n">
         <v>0</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Mut</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Minimal</t>
-        </is>
-      </c>
-      <c r="D3">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="n">
         <v>13.625</v>
       </c>
-      <c r="E3">
-        <v>6.549491074376187</v>
+      <c r="E3" t="n">
+        <v>6.54949107437619</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4">
+      <c r="A4" t="n">
         <v>0</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>WT</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>LB</t>
-        </is>
-      </c>
-      <c r="D4">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="n">
         <v>9.5</v>
       </c>
-      <c r="E4">
-        <v>8.062257748298549</v>
+      <c r="E4" t="n">
+        <v>8.06225774829855</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5">
+      <c r="A5" t="n">
         <v>0</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>WT</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Minimal</t>
-        </is>
-      </c>
-      <c r="D5">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="n">
         <v>13.75</v>
       </c>
-      <c r="E5">
-        <v>6.614378277661476</v>
+      <c r="E5" t="n">
+        <v>6.61437827766148</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Mut</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>LB</t>
-        </is>
-      </c>
-      <c r="D6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="n">
         <v>4.02021808267937</v>
       </c>
-      <c r="E6">
-        <v>0.7467461347877933</v>
+      <c r="E6" t="n">
+        <v>0.746746134787793</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Mut</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Minimal</t>
-        </is>
-      </c>
-      <c r="D7">
-        <v>8.886318464490484</v>
-      </c>
-      <c r="E7">
-        <v>1.807907959127571</v>
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="n">
+        <v>8.88631846449048</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.80790795912757</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>WT</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>LB</t>
-        </is>
-      </c>
-      <c r="D8">
+      <c r="A8" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="n">
         <v>20.4868473330927</v>
       </c>
-      <c r="E8">
-        <v>2.225449971512377</v>
+      <c r="E8" t="n">
+        <v>2.22544997151238</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9">
-        <v>5</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>WT</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Minimal</t>
-        </is>
-      </c>
-      <c r="D9">
-        <v>49.37348356296913</v>
-      </c>
-      <c r="E9">
-        <v>9.653855203929876</v>
+      <c r="A9" t="n">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="n">
+        <v>49.3734835629691</v>
+      </c>
+      <c r="E9" t="n">
+        <v>9.65385520392988</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10">
+      <c r="A10" t="n">
         <v>10</v>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Mut</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>LB</t>
-        </is>
-      </c>
-      <c r="D10">
-        <v>1.708177031893257</v>
-      </c>
-      <c r="E10">
-        <v>0.3703988344990392</v>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1.70817703189326</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.370398834499039</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11">
+      <c r="A11" t="n">
         <v>10</v>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Mut</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Minimal</t>
-        </is>
-      </c>
-      <c r="D11">
-        <v>3.830043859649123</v>
-      </c>
-      <c r="E11">
-        <v>0.6914574881994361</v>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="n">
+        <v>3.83004385964912</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.691457488199436</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12">
+      <c r="A12" t="n">
         <v>10</v>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>WT</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>LB</t>
-        </is>
-      </c>
-      <c r="D12">
-        <v>24.27388915432394</v>
-      </c>
-      <c r="E12">
-        <v>3.432862562929507</v>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="n">
+        <v>24.2738891543239</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3.43286256292951</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13">
+      <c r="A13" t="n">
         <v>10</v>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>WT</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Minimal</t>
-        </is>
-      </c>
-      <c r="D13">
-        <v>47.60796373296373</v>
-      </c>
-      <c r="E13">
-        <v>5.422272880594172</v>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="n">
+        <v>47.6079637329637</v>
+      </c>
+      <c r="E13" t="n">
+        <v>5.42227288059417</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>